<commit_message>
modules / glue script to add curated data.
</commit_message>
<xml_diff>
--- a/tabular/1. BTV DB all segs 2016-06-17 seq to delete.xlsx
+++ b/tabular/1. BTV DB all segs 2016-06-17 seq to delete.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="266">
   <si>
     <t>gb_primary_accession</t>
   </si>
@@ -814,13 +814,16 @@
   </si>
   <si>
     <t>sequence_id</t>
+  </si>
+  <si>
+    <t>excluded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -850,6 +853,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -868,7 +878,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="977">
+  <cellStyleXfs count="993">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1846,8 +1856,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1858,8 +1884,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="977">
+  <cellStyles count="993">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2348,6 +2375,14 @@
     <cellStyle name="Followed Hyperlink" xfId="972" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="974" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="976" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="992" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2836,6 +2871,14 @@
     <cellStyle name="Hyperlink" xfId="971" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="973" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="975" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="991" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3165,11 +3208,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T120"/>
+  <dimension ref="A1:U120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U28" sqref="U28:U120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3183,7 +3226,7 @@
     <col min="21" max="21" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>264</v>
       </c>
@@ -3244,8 +3287,11 @@
       <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3306,8 +3352,11 @@
       <c r="T2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3368,8 +3417,11 @@
       <c r="T3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3430,8 +3482,11 @@
       <c r="T4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3492,8 +3547,11 @@
       <c r="T5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3554,8 +3612,11 @@
       <c r="T6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3616,8 +3677,11 @@
       <c r="T7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" s="4" customFormat="1">
+      <c r="U7" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="4" customFormat="1">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3678,8 +3742,11 @@
       <c r="T8" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" s="4" customFormat="1">
+      <c r="U8" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="4" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
@@ -3740,8 +3807,11 @@
       <c r="T9" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" s="4" customFormat="1">
+      <c r="U9" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="4" customFormat="1">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
@@ -3802,8 +3872,11 @@
       <c r="T10" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" s="4" customFormat="1">
+      <c r="U10" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="4" customFormat="1">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -3864,8 +3937,11 @@
       <c r="T11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" s="4" customFormat="1">
+      <c r="U11" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="4" customFormat="1">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -3926,8 +4002,11 @@
       <c r="T12" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" s="4" customFormat="1">
+      <c r="U12" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="4" customFormat="1">
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
@@ -3988,8 +4067,11 @@
       <c r="T13" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" s="4" customFormat="1">
+      <c r="U13" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -4050,8 +4132,11 @@
       <c r="T14" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" s="4" customFormat="1">
+      <c r="U14" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="4" customFormat="1">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -4112,8 +4197,11 @@
       <c r="T15" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" s="4" customFormat="1">
+      <c r="U15" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="4" customFormat="1">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -4174,8 +4262,11 @@
       <c r="T16" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" s="4" customFormat="1">
+      <c r="U16" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="4" customFormat="1">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -4236,8 +4327,11 @@
       <c r="T17" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" s="4" customFormat="1">
+      <c r="U17" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="4" customFormat="1">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -4298,8 +4392,11 @@
       <c r="T18" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" s="4" customFormat="1">
+      <c r="U18" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="4" customFormat="1">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -4360,8 +4457,11 @@
       <c r="T19" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" s="4" customFormat="1">
+      <c r="U19" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="4" customFormat="1">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -4422,8 +4522,11 @@
       <c r="T20" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" s="4" customFormat="1">
+      <c r="U20" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="4" customFormat="1">
       <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
@@ -4484,8 +4587,11 @@
       <c r="T21" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" s="4" customFormat="1">
+      <c r="U21" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="4" customFormat="1">
       <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
@@ -4546,8 +4652,11 @@
       <c r="T22" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" s="4" customFormat="1">
+      <c r="U22" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="4" customFormat="1">
       <c r="A23" s="4" t="s">
         <v>57</v>
       </c>
@@ -4608,8 +4717,11 @@
       <c r="T23" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" s="4" customFormat="1">
+      <c r="U23" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="4" customFormat="1">
       <c r="A24" s="4" t="s">
         <v>59</v>
       </c>
@@ -4670,8 +4782,11 @@
       <c r="T24" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" s="4" customFormat="1">
+      <c r="U24" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="4" customFormat="1">
       <c r="A25" s="4" t="s">
         <v>61</v>
       </c>
@@ -4732,8 +4847,11 @@
       <c r="T25" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" s="4" customFormat="1">
+      <c r="U25" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="4" customFormat="1">
       <c r="A26" s="4" t="s">
         <v>63</v>
       </c>
@@ -4794,8 +4912,11 @@
       <c r="T26" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" s="4" customFormat="1">
+      <c r="U26" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="4" customFormat="1">
       <c r="A27" s="4" t="s">
         <v>65</v>
       </c>
@@ -4856,8 +4977,11 @@
       <c r="T27" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" s="4" customFormat="1">
+      <c r="U27" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="4" customFormat="1">
       <c r="A28" s="4" t="s">
         <v>67</v>
       </c>
@@ -4918,8 +5042,11 @@
       <c r="T28" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" s="4" customFormat="1">
+      <c r="U28" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="4" customFormat="1">
       <c r="A29" s="4" t="s">
         <v>69</v>
       </c>
@@ -4980,8 +5107,11 @@
       <c r="T29" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" s="4" customFormat="1">
+      <c r="U29" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="4" customFormat="1">
       <c r="A30" s="4" t="s">
         <v>71</v>
       </c>
@@ -5042,8 +5172,11 @@
       <c r="T30" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" s="4" customFormat="1">
+      <c r="U30" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="4" customFormat="1">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
@@ -5104,8 +5237,11 @@
       <c r="T31" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" s="4" customFormat="1">
+      <c r="U31" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="4" customFormat="1">
       <c r="A32" s="4" t="s">
         <v>75</v>
       </c>
@@ -5166,8 +5302,11 @@
       <c r="T32" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" s="4" customFormat="1">
+      <c r="U32" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="4" customFormat="1">
       <c r="A33" s="4" t="s">
         <v>79</v>
       </c>
@@ -5228,8 +5367,11 @@
       <c r="T33" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" s="4" customFormat="1">
+      <c r="U33" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" s="4" customFormat="1">
       <c r="A34" s="4" t="s">
         <v>82</v>
       </c>
@@ -5290,8 +5432,11 @@
       <c r="T34" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" s="4" customFormat="1">
+      <c r="U34" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="4" customFormat="1">
       <c r="A35" s="4" t="s">
         <v>84</v>
       </c>
@@ -5352,8 +5497,11 @@
       <c r="T35" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" s="4" customFormat="1">
+      <c r="U35" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" s="4" customFormat="1">
       <c r="A36" s="4" t="s">
         <v>86</v>
       </c>
@@ -5414,8 +5562,11 @@
       <c r="T36" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" s="4" customFormat="1">
+      <c r="U36" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" s="4" customFormat="1">
       <c r="A37" s="4" t="s">
         <v>91</v>
       </c>
@@ -5476,8 +5627,11 @@
       <c r="T37" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" s="4" customFormat="1">
+      <c r="U37" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" s="4" customFormat="1">
       <c r="A38" s="4" t="s">
         <v>94</v>
       </c>
@@ -5538,8 +5692,11 @@
       <c r="T38" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" s="4" customFormat="1">
+      <c r="U38" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" s="4" customFormat="1">
       <c r="A39" s="4" t="s">
         <v>96</v>
       </c>
@@ -5600,8 +5757,11 @@
       <c r="T39" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" s="4" customFormat="1">
+      <c r="U39" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" s="4" customFormat="1">
       <c r="A40" s="4" t="s">
         <v>98</v>
       </c>
@@ -5662,8 +5822,11 @@
       <c r="T40" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" s="4" customFormat="1">
+      <c r="U40" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" s="4" customFormat="1">
       <c r="A41" s="4" t="s">
         <v>100</v>
       </c>
@@ -5724,8 +5887,11 @@
       <c r="T41" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" s="4" customFormat="1">
+      <c r="U41" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" s="4" customFormat="1">
       <c r="A42" s="4" t="s">
         <v>102</v>
       </c>
@@ -5786,8 +5952,11 @@
       <c r="T42" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" s="4" customFormat="1">
+      <c r="U42" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" s="4" customFormat="1">
       <c r="A43" s="4" t="s">
         <v>104</v>
       </c>
@@ -5848,8 +6017,11 @@
       <c r="T43" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" s="4" customFormat="1">
+      <c r="U43" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" s="4" customFormat="1">
       <c r="A44" s="4" t="s">
         <v>106</v>
       </c>
@@ -5910,8 +6082,11 @@
       <c r="T44" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" s="4" customFormat="1">
+      <c r="U44" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" s="4" customFormat="1">
       <c r="A45" s="4" t="s">
         <v>108</v>
       </c>
@@ -5972,8 +6147,11 @@
       <c r="T45" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" s="4" customFormat="1">
+      <c r="U45" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" s="4" customFormat="1">
       <c r="A46" s="4" t="s">
         <v>110</v>
       </c>
@@ -6034,8 +6212,11 @@
       <c r="T46" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" s="4" customFormat="1">
+      <c r="U46" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" s="4" customFormat="1">
       <c r="A47" s="4" t="s">
         <v>112</v>
       </c>
@@ -6096,8 +6277,11 @@
       <c r="T47" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" s="4" customFormat="1">
+      <c r="U47" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" s="4" customFormat="1">
       <c r="A48" s="4" t="s">
         <v>114</v>
       </c>
@@ -6158,8 +6342,11 @@
       <c r="T48" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" s="4" customFormat="1">
+      <c r="U48" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" s="4" customFormat="1">
       <c r="A49" s="4" t="s">
         <v>116</v>
       </c>
@@ -6220,8 +6407,11 @@
       <c r="T49" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" s="4" customFormat="1">
+      <c r="U49" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" s="4" customFormat="1">
       <c r="A50" s="4" t="s">
         <v>118</v>
       </c>
@@ -6282,8 +6472,11 @@
       <c r="T50" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" s="4" customFormat="1">
+      <c r="U50" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" s="4" customFormat="1">
       <c r="A51" s="4" t="s">
         <v>120</v>
       </c>
@@ -6344,8 +6537,11 @@
       <c r="T51" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" s="4" customFormat="1">
+      <c r="U51" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" s="4" customFormat="1">
       <c r="A52" s="4" t="s">
         <v>122</v>
       </c>
@@ -6406,8 +6602,11 @@
       <c r="T52" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" s="4" customFormat="1">
+      <c r="U52" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" s="4" customFormat="1">
       <c r="A53" s="4" t="s">
         <v>124</v>
       </c>
@@ -6468,8 +6667,11 @@
       <c r="T53" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" s="4" customFormat="1">
+      <c r="U53" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" s="4" customFormat="1">
       <c r="A54" s="4" t="s">
         <v>126</v>
       </c>
@@ -6530,8 +6732,11 @@
       <c r="T54" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" s="4" customFormat="1">
+      <c r="U54" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" s="4" customFormat="1">
       <c r="A55" s="4" t="s">
         <v>128</v>
       </c>
@@ -6592,8 +6797,11 @@
       <c r="T55" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" s="4" customFormat="1">
+      <c r="U55" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" s="4" customFormat="1">
       <c r="A56" s="4" t="s">
         <v>130</v>
       </c>
@@ -6654,8 +6862,11 @@
       <c r="T56" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" s="4" customFormat="1">
+      <c r="U56" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" s="4" customFormat="1">
       <c r="A57" s="4" t="s">
         <v>132</v>
       </c>
@@ -6716,8 +6927,11 @@
       <c r="T57" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" s="4" customFormat="1">
+      <c r="U57" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" s="4" customFormat="1">
       <c r="A58" s="4" t="s">
         <v>134</v>
       </c>
@@ -6778,8 +6992,11 @@
       <c r="T58" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" s="4" customFormat="1">
+      <c r="U58" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" s="4" customFormat="1">
       <c r="A59" s="4" t="s">
         <v>136</v>
       </c>
@@ -6840,8 +7057,11 @@
       <c r="T59" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" s="4" customFormat="1">
+      <c r="U59" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" s="4" customFormat="1">
       <c r="A60" s="4" t="s">
         <v>138</v>
       </c>
@@ -6902,8 +7122,11 @@
       <c r="T60" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" s="4" customFormat="1">
+      <c r="U60" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" s="4" customFormat="1">
       <c r="A61" s="4" t="s">
         <v>140</v>
       </c>
@@ -6964,8 +7187,11 @@
       <c r="T61" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" s="4" customFormat="1">
+      <c r="U61" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" s="4" customFormat="1">
       <c r="A62" s="4" t="s">
         <v>142</v>
       </c>
@@ -7026,8 +7252,11 @@
       <c r="T62" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" s="4" customFormat="1">
+      <c r="U62" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" s="4" customFormat="1">
       <c r="A63" s="4" t="s">
         <v>144</v>
       </c>
@@ -7088,8 +7317,11 @@
       <c r="T63" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" s="4" customFormat="1">
+      <c r="U63" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" s="4" customFormat="1">
       <c r="A64" s="4" t="s">
         <v>146</v>
       </c>
@@ -7150,8 +7382,11 @@
       <c r="T64" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" s="4" customFormat="1">
+      <c r="U64" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" s="4" customFormat="1">
       <c r="A65" s="4" t="s">
         <v>148</v>
       </c>
@@ -7212,8 +7447,11 @@
       <c r="T65" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" s="4" customFormat="1">
+      <c r="U65" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" s="4" customFormat="1">
       <c r="A66" s="4" t="s">
         <v>150</v>
       </c>
@@ -7274,8 +7512,11 @@
       <c r="T66" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" s="4" customFormat="1">
+      <c r="U66" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" s="4" customFormat="1">
       <c r="A67" s="4" t="s">
         <v>154</v>
       </c>
@@ -7336,8 +7577,11 @@
       <c r="T67" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" s="4" customFormat="1">
+      <c r="U67" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" s="4" customFormat="1">
       <c r="A68" s="4" t="s">
         <v>156</v>
       </c>
@@ -7398,8 +7642,11 @@
       <c r="T68" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="69" spans="1:20" s="4" customFormat="1">
+      <c r="U68" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" s="4" customFormat="1">
       <c r="A69" s="4" t="s">
         <v>158</v>
       </c>
@@ -7460,8 +7707,11 @@
       <c r="T69" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" s="4" customFormat="1">
+      <c r="U69" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" s="4" customFormat="1">
       <c r="A70" s="4" t="s">
         <v>160</v>
       </c>
@@ -7522,8 +7772,11 @@
       <c r="T70" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" s="4" customFormat="1">
+      <c r="U70" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" s="4" customFormat="1">
       <c r="A71" s="4" t="s">
         <v>162</v>
       </c>
@@ -7584,8 +7837,11 @@
       <c r="T71" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" s="4" customFormat="1">
+      <c r="U71" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" s="4" customFormat="1">
       <c r="A72" s="4" t="s">
         <v>164</v>
       </c>
@@ -7646,8 +7902,11 @@
       <c r="T72" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="73" spans="1:20" s="4" customFormat="1">
+      <c r="U72" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" s="4" customFormat="1">
       <c r="A73" s="4" t="s">
         <v>166</v>
       </c>
@@ -7708,8 +7967,11 @@
       <c r="T73" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" s="4" customFormat="1">
+      <c r="U73" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" s="4" customFormat="1">
       <c r="A74" s="4" t="s">
         <v>168</v>
       </c>
@@ -7770,8 +8032,11 @@
       <c r="T74" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" s="4" customFormat="1">
+      <c r="U74" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" s="4" customFormat="1">
       <c r="A75" s="4" t="s">
         <v>170</v>
       </c>
@@ -7832,8 +8097,11 @@
       <c r="T75" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" s="4" customFormat="1">
+      <c r="U75" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" s="4" customFormat="1">
       <c r="A76" s="4" t="s">
         <v>172</v>
       </c>
@@ -7894,8 +8162,11 @@
       <c r="T76" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" s="4" customFormat="1">
+      <c r="U76" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" s="4" customFormat="1">
       <c r="A77" s="4" t="s">
         <v>174</v>
       </c>
@@ -7956,8 +8227,11 @@
       <c r="T77" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="78" spans="1:20" s="4" customFormat="1">
+      <c r="U77" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="4" customFormat="1">
       <c r="A78" s="4" t="s">
         <v>176</v>
       </c>
@@ -8018,8 +8292,11 @@
       <c r="T78" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="79" spans="1:20" s="4" customFormat="1">
+      <c r="U78" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="4" customFormat="1">
       <c r="A79" s="4" t="s">
         <v>178</v>
       </c>
@@ -8080,8 +8357,11 @@
       <c r="T79" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="80" spans="1:20" s="4" customFormat="1">
+      <c r="U79" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="4" customFormat="1">
       <c r="A80" s="4" t="s">
         <v>180</v>
       </c>
@@ -8142,8 +8422,11 @@
       <c r="T80" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" s="4" customFormat="1">
+      <c r="U80" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" s="4" customFormat="1">
       <c r="A81" s="4" t="s">
         <v>182</v>
       </c>
@@ -8204,8 +8487,11 @@
       <c r="T81" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" s="4" customFormat="1">
+      <c r="U81" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" s="4" customFormat="1">
       <c r="A82" s="4" t="s">
         <v>184</v>
       </c>
@@ -8266,8 +8552,11 @@
       <c r="T82" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" s="4" customFormat="1">
+      <c r="U82" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" s="4" customFormat="1">
       <c r="A83" s="4" t="s">
         <v>186</v>
       </c>
@@ -8328,8 +8617,11 @@
       <c r="T83" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" s="4" customFormat="1">
+      <c r="U83" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" s="4" customFormat="1">
       <c r="A84" s="4" t="s">
         <v>188</v>
       </c>
@@ -8390,8 +8682,11 @@
       <c r="T84" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="85" spans="1:20" s="4" customFormat="1">
+      <c r="U84" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" s="4" customFormat="1">
       <c r="A85" s="4" t="s">
         <v>190</v>
       </c>
@@ -8452,8 +8747,11 @@
       <c r="T85" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="86" spans="1:20" s="4" customFormat="1">
+      <c r="U85" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" s="4" customFormat="1">
       <c r="A86" s="4" t="s">
         <v>192</v>
       </c>
@@ -8514,8 +8812,11 @@
       <c r="T86" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="87" spans="1:20" s="4" customFormat="1">
+      <c r="U86" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" s="4" customFormat="1">
       <c r="A87" s="4" t="s">
         <v>194</v>
       </c>
@@ -8576,8 +8877,11 @@
       <c r="T87" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="88" spans="1:20" s="4" customFormat="1">
+      <c r="U87" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" s="4" customFormat="1">
       <c r="A88" s="4" t="s">
         <v>196</v>
       </c>
@@ -8638,8 +8942,11 @@
       <c r="T88" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" s="4" customFormat="1">
+      <c r="U88" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" s="4" customFormat="1">
       <c r="A89" s="4" t="s">
         <v>198</v>
       </c>
@@ -8700,8 +9007,11 @@
       <c r="T89" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="90" spans="1:20" s="4" customFormat="1">
+      <c r="U89" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" s="4" customFormat="1">
       <c r="A90" s="4" t="s">
         <v>200</v>
       </c>
@@ -8762,8 +9072,11 @@
       <c r="T90" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="91" spans="1:20" s="4" customFormat="1">
+      <c r="U90" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" s="4" customFormat="1">
       <c r="A91" s="4" t="s">
         <v>202</v>
       </c>
@@ -8824,8 +9137,11 @@
       <c r="T91" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:20" s="4" customFormat="1">
+      <c r="U91" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" s="4" customFormat="1">
       <c r="A92" s="4" t="s">
         <v>204</v>
       </c>
@@ -8886,8 +9202,11 @@
       <c r="T92" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="93" spans="1:20" s="4" customFormat="1">
+      <c r="U92" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" s="4" customFormat="1">
       <c r="A93" s="4" t="s">
         <v>206</v>
       </c>
@@ -8948,8 +9267,11 @@
       <c r="T93" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="94" spans="1:20" s="4" customFormat="1">
+      <c r="U93" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" s="4" customFormat="1">
       <c r="A94" s="4" t="s">
         <v>208</v>
       </c>
@@ -9010,8 +9332,11 @@
       <c r="T94" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="95" spans="1:20" s="4" customFormat="1">
+      <c r="U94" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" s="4" customFormat="1">
       <c r="A95" s="4" t="s">
         <v>210</v>
       </c>
@@ -9072,8 +9397,11 @@
       <c r="T95" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="96" spans="1:20" s="4" customFormat="1">
+      <c r="U95" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" s="4" customFormat="1">
       <c r="A96" s="4" t="s">
         <v>212</v>
       </c>
@@ -9134,8 +9462,11 @@
       <c r="T96" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="97" spans="1:20" s="4" customFormat="1">
+      <c r="U96" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" s="4" customFormat="1">
       <c r="A97" s="4" t="s">
         <v>214</v>
       </c>
@@ -9196,8 +9527,11 @@
       <c r="T97" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="98" spans="1:20" s="4" customFormat="1">
+      <c r="U97" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" s="4" customFormat="1">
       <c r="A98" s="4" t="s">
         <v>216</v>
       </c>
@@ -9258,8 +9592,11 @@
       <c r="T98" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="99" spans="1:20" s="4" customFormat="1">
+      <c r="U98" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" s="4" customFormat="1">
       <c r="A99" s="4" t="s">
         <v>218</v>
       </c>
@@ -9320,8 +9657,11 @@
       <c r="T99" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="100" spans="1:20" s="4" customFormat="1">
+      <c r="U99" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" s="4" customFormat="1">
       <c r="A100" s="4" t="s">
         <v>220</v>
       </c>
@@ -9382,8 +9722,11 @@
       <c r="T100" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="101" spans="1:20" s="4" customFormat="1">
+      <c r="U100" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" s="4" customFormat="1">
       <c r="A101" s="4" t="s">
         <v>222</v>
       </c>
@@ -9444,8 +9787,11 @@
       <c r="T101" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:20" s="4" customFormat="1">
+      <c r="U101" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" s="4" customFormat="1">
       <c r="A102" s="4" t="s">
         <v>224</v>
       </c>
@@ -9506,8 +9852,11 @@
       <c r="T102" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="103" spans="1:20" s="4" customFormat="1">
+      <c r="U102" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" s="4" customFormat="1">
       <c r="A103" s="4" t="s">
         <v>226</v>
       </c>
@@ -9568,8 +9917,11 @@
       <c r="T103" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="104" spans="1:20" s="4" customFormat="1">
+      <c r="U103" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" s="4" customFormat="1">
       <c r="A104" s="4" t="s">
         <v>228</v>
       </c>
@@ -9630,8 +9982,11 @@
       <c r="T104" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="105" spans="1:20" s="4" customFormat="1">
+      <c r="U104" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" s="4" customFormat="1">
       <c r="A105" s="4" t="s">
         <v>230</v>
       </c>
@@ -9692,8 +10047,11 @@
       <c r="T105" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="106" spans="1:20" s="4" customFormat="1">
+      <c r="U105" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" s="4" customFormat="1">
       <c r="A106" s="4" t="s">
         <v>232</v>
       </c>
@@ -9754,8 +10112,11 @@
       <c r="T106" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:20" s="4" customFormat="1">
+      <c r="U106" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" s="4" customFormat="1">
       <c r="A107" s="4" t="s">
         <v>234</v>
       </c>
@@ -9816,8 +10177,11 @@
       <c r="T107" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="108" spans="1:20" s="4" customFormat="1">
+      <c r="U107" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" s="4" customFormat="1">
       <c r="A108" s="4" t="s">
         <v>236</v>
       </c>
@@ -9878,8 +10242,11 @@
       <c r="T108" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="109" spans="1:20" s="4" customFormat="1">
+      <c r="U108" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" s="4" customFormat="1">
       <c r="A109" s="4" t="s">
         <v>238</v>
       </c>
@@ -9940,8 +10307,11 @@
       <c r="T109" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="110" spans="1:20" s="4" customFormat="1">
+      <c r="U109" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" s="4" customFormat="1">
       <c r="A110" s="4" t="s">
         <v>240</v>
       </c>
@@ -10002,8 +10372,11 @@
       <c r="T110" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="111" spans="1:20" s="4" customFormat="1">
+      <c r="U110" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" s="4" customFormat="1">
       <c r="A111" s="4" t="s">
         <v>242</v>
       </c>
@@ -10064,8 +10437,11 @@
       <c r="T111" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="112" spans="1:20" s="4" customFormat="1">
+      <c r="U111" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" s="4" customFormat="1">
       <c r="A112" s="4" t="s">
         <v>244</v>
       </c>
@@ -10126,8 +10502,11 @@
       <c r="T112" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="113" spans="1:20" s="4" customFormat="1">
+      <c r="U112" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" s="4" customFormat="1">
       <c r="A113" s="4" t="s">
         <v>246</v>
       </c>
@@ -10188,8 +10567,11 @@
       <c r="T113" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="114" spans="1:20" s="4" customFormat="1">
+      <c r="U113" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" s="4" customFormat="1">
       <c r="A114" s="4" t="s">
         <v>248</v>
       </c>
@@ -10250,8 +10632,11 @@
       <c r="T114" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="115" spans="1:20" s="4" customFormat="1">
+      <c r="U114" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" s="4" customFormat="1">
       <c r="A115" s="4" t="s">
         <v>250</v>
       </c>
@@ -10312,8 +10697,11 @@
       <c r="T115" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="116" spans="1:20" s="4" customFormat="1">
+      <c r="U115" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" s="4" customFormat="1">
       <c r="A116" s="4" t="s">
         <v>252</v>
       </c>
@@ -10374,8 +10762,11 @@
       <c r="T116" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="117" spans="1:20" s="4" customFormat="1">
+      <c r="U116" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" s="4" customFormat="1">
       <c r="A117" s="4" t="s">
         <v>254</v>
       </c>
@@ -10436,8 +10827,11 @@
       <c r="T117" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="118" spans="1:20" s="4" customFormat="1">
+      <c r="U117" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" s="4" customFormat="1">
       <c r="A118" s="4" t="s">
         <v>256</v>
       </c>
@@ -10498,8 +10892,11 @@
       <c r="T118" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="119" spans="1:20" s="4" customFormat="1">
+      <c r="U118" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" s="4" customFormat="1">
       <c r="A119" s="4" t="s">
         <v>258</v>
       </c>
@@ -10560,8 +10957,11 @@
       <c r="T119" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="120" spans="1:20" s="4" customFormat="1">
+      <c r="U119" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" s="4" customFormat="1">
       <c r="A120" s="4" t="s">
         <v>260</v>
       </c>
@@ -10621,6 +11021,9 @@
       </c>
       <c r="T120" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="U120" s="6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>